<commit_message>
feat: add all output graphs and updated readme
</commit_message>
<xml_diff>
--- a/Chart Run Log.xlsx
+++ b/Chart Run Log.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\artbo\Desktop\ml-stock-predictions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4568090D-687E-4DE4-A534-F4637FED6164}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3272AC7-3749-44D9-8391-2844C41C208F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="30" windowWidth="14715" windowHeight="11700" xr2:uid="{E8AD1043-31C5-4B0E-86AF-5973CED729A2}"/>
+    <workbookView xWindow="180" yWindow="330" windowWidth="16440" windowHeight="16305" xr2:uid="{E8AD1043-31C5-4B0E-86AF-5973CED729A2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$30</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="16">
   <si>
     <t>RMSE</t>
   </si>
@@ -42,37 +45,46 @@
     <t>Epochs</t>
   </si>
   <si>
-    <t>LSTM</t>
-  </si>
-  <si>
-    <t>Dense</t>
-  </si>
-  <si>
-    <t>Dropout</t>
-  </si>
-  <si>
     <t>Batch Size</t>
   </si>
   <si>
-    <t>LookBack</t>
-  </si>
-  <si>
-    <t>Time</t>
-  </si>
-  <si>
     <t>2(50)</t>
   </si>
   <si>
     <t>1(1)</t>
   </si>
   <si>
-    <t>Run</t>
-  </si>
-  <si>
     <t>3(50)</t>
   </si>
   <si>
     <t>2(20/1)</t>
+  </si>
+  <si>
+    <t>4(50)</t>
+  </si>
+  <si>
+    <t>4 (LSTM &amp; Dense)</t>
+  </si>
+  <si>
+    <t>3 (LSTM Only)</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>Dropout Layers</t>
+  </si>
+  <si>
+    <t>Dense Layers</t>
+  </si>
+  <si>
+    <t>LSTM Layers</t>
+  </si>
+  <si>
+    <t>Run Time</t>
+  </si>
+  <si>
+    <t>Run #</t>
   </si>
 </sst>
 </file>
@@ -88,8 +100,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFD4D4D4"/>
+      <sz val="9"/>
+      <color rgb="FF032F62"/>
       <name val="Consolas"/>
       <family val="3"/>
     </font>
@@ -431,24 +443,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E73BDE7-615B-47AA-9A27-BDFA30A5202D}">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="16.7109375" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" customWidth="1"/>
+    <col min="4" max="8" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -457,22 +470,19 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="G1" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="H1" t="s">
-        <v>4</v>
-      </c>
-      <c r="I1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -489,19 +499,16 @@
         <v>32</v>
       </c>
       <c r="F2" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -518,19 +525,16 @@
         <v>32</v>
       </c>
       <c r="F3" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -547,19 +551,16 @@
         <v>32</v>
       </c>
       <c r="F4" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G4" t="s">
-        <v>9</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -576,19 +577,16 @@
         <v>32</v>
       </c>
       <c r="F5" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -605,19 +603,16 @@
         <v>32</v>
       </c>
       <c r="F6" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-      <c r="I6">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -634,19 +629,16 @@
         <v>16</v>
       </c>
       <c r="F7" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G7" t="s">
-        <v>9</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -663,19 +655,16 @@
         <v>16</v>
       </c>
       <c r="F8" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G8" t="s">
-        <v>9</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -692,24 +681,22 @@
         <v>16</v>
       </c>
       <c r="F9" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G9" t="s">
-        <v>9</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H9" t="s">
+        <v>10</v>
+      </c>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10">
-        <v>25</v>
+        <v>0.25</v>
       </c>
       <c r="C10">
         <v>14.102921931365399</v>
@@ -721,19 +708,16 @@
         <v>64</v>
       </c>
       <c r="F10" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G10" t="s">
-        <v>9</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -750,19 +734,16 @@
         <v>64</v>
       </c>
       <c r="F11" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G11" t="s">
-        <v>9</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="I11">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -779,26 +760,23 @@
         <v>64</v>
       </c>
       <c r="F12" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G12" t="s">
-        <v>9</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
       <c r="B13">
         <v>0.44</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13">
         <v>7.05807729783628</v>
       </c>
       <c r="D13">
@@ -808,26 +786,23 @@
         <v>32</v>
       </c>
       <c r="F13" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="G13" t="s">
-        <v>9</v>
-      </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-      <c r="I13">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14">
         <v>2.39</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14">
         <v>9.3121118279283195</v>
       </c>
       <c r="D14">
@@ -837,26 +812,23 @@
         <v>32</v>
       </c>
       <c r="F14" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="G14" t="s">
-        <v>9</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-      <c r="I14">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15">
         <v>5</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15">
         <v>7.10921982812118</v>
       </c>
       <c r="D15">
@@ -866,26 +838,23 @@
         <v>32</v>
       </c>
       <c r="F15" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="G15" t="s">
-        <v>9</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-      <c r="I15">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="H15" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16">
         <v>0.33</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16">
         <v>7.7122696299234104</v>
       </c>
       <c r="D16">
@@ -895,26 +864,23 @@
         <v>32</v>
       </c>
       <c r="F16" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G16" t="s">
-        <v>12</v>
-      </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
-      <c r="I16">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="H16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
       <c r="B17">
         <v>1.49</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17">
         <v>6.3031113153608</v>
       </c>
       <c r="D17">
@@ -924,26 +890,23 @@
         <v>32</v>
       </c>
       <c r="F17" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="G17" t="s">
-        <v>12</v>
-      </c>
-      <c r="H17">
-        <v>0</v>
-      </c>
-      <c r="I17">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="H17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
       <c r="B18">
         <v>3.28</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18">
         <v>11.5380523520555</v>
       </c>
       <c r="D18">
@@ -953,19 +916,359 @@
         <v>32</v>
       </c>
       <c r="F18" t="s">
+        <v>3</v>
+      </c>
+      <c r="G18" t="s">
+        <v>6</v>
+      </c>
+      <c r="H18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>0.48</v>
+      </c>
+      <c r="C19">
+        <v>9.72141042076343</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>32</v>
+      </c>
+      <c r="F19" t="s">
+        <v>5</v>
+      </c>
+      <c r="G19" t="s">
+        <v>6</v>
+      </c>
+      <c r="H19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="C20">
+        <v>8.79276109662983</v>
+      </c>
+      <c r="D20">
+        <v>5</v>
+      </c>
+      <c r="E20">
+        <v>32</v>
+      </c>
+      <c r="F20" t="s">
+        <v>5</v>
+      </c>
+      <c r="G20" t="s">
+        <v>6</v>
+      </c>
+      <c r="H20" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>5.03</v>
+      </c>
+      <c r="C21">
+        <v>5.9469095370263902</v>
+      </c>
+      <c r="D21">
+        <v>10</v>
+      </c>
+      <c r="E21">
+        <v>32</v>
+      </c>
+      <c r="F21" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21" t="s">
+        <v>6</v>
+      </c>
+      <c r="H21" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>1.02</v>
+      </c>
+      <c r="C22">
+        <v>11.8427285208426</v>
+      </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>32</v>
+      </c>
+      <c r="F22" t="s">
+        <v>7</v>
+      </c>
+      <c r="G22" t="s">
+        <v>6</v>
+      </c>
+      <c r="H22" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>3.32</v>
+      </c>
+      <c r="C23">
+        <v>7.3307571232445001</v>
+      </c>
+      <c r="D23">
+        <v>5</v>
+      </c>
+      <c r="E23">
+        <v>32</v>
+      </c>
+      <c r="F23" t="s">
+        <v>7</v>
+      </c>
+      <c r="G23" t="s">
+        <v>6</v>
+      </c>
+      <c r="H23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>6.53</v>
+      </c>
+      <c r="C24">
+        <v>11.436490027869</v>
+      </c>
+      <c r="D24">
+        <v>10</v>
+      </c>
+      <c r="E24">
+        <v>32</v>
+      </c>
+      <c r="F24" t="s">
+        <v>7</v>
+      </c>
+      <c r="G24" t="s">
+        <v>6</v>
+      </c>
+      <c r="H24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>0.45</v>
+      </c>
+      <c r="C25">
+        <v>6.8942337876372797</v>
+      </c>
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>32</v>
+      </c>
+      <c r="F25" t="s">
+        <v>5</v>
+      </c>
+      <c r="G25" t="s">
+        <v>6</v>
+      </c>
+      <c r="H25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>2.42</v>
+      </c>
+      <c r="C26">
+        <v>8.6886668808455205</v>
+      </c>
+      <c r="D26">
+        <v>5</v>
+      </c>
+      <c r="E26">
+        <v>32</v>
+      </c>
+      <c r="F26" t="s">
+        <v>5</v>
+      </c>
+      <c r="G26" t="s">
+        <v>6</v>
+      </c>
+      <c r="H26" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>5.36</v>
+      </c>
+      <c r="C27">
+        <v>9.5091007888136403</v>
+      </c>
+      <c r="D27">
+        <v>10</v>
+      </c>
+      <c r="E27">
+        <v>32</v>
+      </c>
+      <c r="F27" t="s">
+        <v>5</v>
+      </c>
+      <c r="G27" t="s">
+        <v>6</v>
+      </c>
+      <c r="H27" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>0.49</v>
+      </c>
+      <c r="C28">
+        <v>9.1983123273659508</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>32</v>
+      </c>
+      <c r="F28" t="s">
+        <v>5</v>
+      </c>
+      <c r="G28" t="s">
+        <v>6</v>
+      </c>
+      <c r="H28" t="s">
         <v>8</v>
       </c>
-      <c r="G18" t="s">
-        <v>12</v>
-      </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
-      <c r="I18">
-        <v>365</v>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>2.5</v>
+      </c>
+      <c r="C29">
+        <v>10.4454339170537</v>
+      </c>
+      <c r="D29">
+        <v>5</v>
+      </c>
+      <c r="E29">
+        <v>32</v>
+      </c>
+      <c r="F29" t="s">
+        <v>5</v>
+      </c>
+      <c r="G29" t="s">
+        <v>6</v>
+      </c>
+      <c r="H29" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>5.25</v>
+      </c>
+      <c r="C30">
+        <v>8.2773318886431202</v>
+      </c>
+      <c r="D30">
+        <v>10</v>
+      </c>
+      <c r="E30">
+        <v>32</v>
+      </c>
+      <c r="F30" t="s">
+        <v>5</v>
+      </c>
+      <c r="G30" t="s">
+        <v>6</v>
+      </c>
+      <c r="H30" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>8.35</v>
+      </c>
+      <c r="C31">
+        <v>7.9376260995514301</v>
+      </c>
+      <c r="D31">
+        <v>10</v>
+      </c>
+      <c r="E31">
+        <v>16</v>
+      </c>
+      <c r="F31" t="s">
+        <v>5</v>
+      </c>
+      <c r="G31" t="s">
+        <v>6</v>
+      </c>
+      <c r="H31" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H30" xr:uid="{7F58C694-8AE9-46DC-A291-5AA997B82616}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H31">
+      <sortCondition ref="A1:A30"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>